<commit_message>
week 3 assignment packages
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-1040" yWindow="460" windowWidth="15520" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="23220" windowHeight="15540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -107,12 +107,6 @@
     <t>[Basic Programming in R II](https://crumplab.github.io/psyc7709/Schedule.html#3_basic_programming_in_r_ii)</t>
   </si>
   <si>
-    <t>[Data-Wrangling](https://crumplab.github.io/psyc7709/Schedule.html#4_data-wrangling)</t>
-  </si>
-  <si>
-    <t>[Data-Visualization](https://crumplab.github.io/psyc7709/Schedule.html#5_data-visualization)</t>
-  </si>
-  <si>
     <t>[Common inferential tests](https://crumplab.github.io/psyc7709/Schedule.html#6_common_inferential_tests)</t>
   </si>
   <si>
@@ -152,12 +146,6 @@
     <t>week 3 due (basics II)</t>
   </si>
   <si>
-    <t>week 4 due (data-wrangling)</t>
-  </si>
-  <si>
-    <t>week 5 due (data-vis)</t>
-  </si>
-  <si>
     <t>week 6 due (stats)</t>
   </si>
   <si>
@@ -180,6 +168,18 @@
   </si>
   <si>
     <t>[Final Project Papers due](https://crumplab.github.io/psyc7709/Schedule.html#15_final_project)</t>
+  </si>
+  <si>
+    <t>[Data-Visualization](https://crumplab.github.io/psyc7709/Schedule.html#4_data-visualization)</t>
+  </si>
+  <si>
+    <t>[Data-Wrangling](https://crumplab.github.io/psyc7709/Schedule.html#5_data-wrangling)</t>
+  </si>
+  <si>
+    <t>week 4 due (data-vis)</t>
+  </si>
+  <si>
+    <t>week 5 due (data-wrangling)</t>
   </si>
 </sst>
 </file>
@@ -499,8 +499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -521,7 +521,7 @@
         <v>18</v>
       </c>
       <c r="D1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="32" x14ac:dyDescent="0.2">
@@ -554,7 +554,7 @@
         <v>24</v>
       </c>
       <c r="D4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="48" x14ac:dyDescent="0.2">
@@ -568,7 +568,7 @@
         <v>25</v>
       </c>
       <c r="D5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -587,10 +587,10 @@
         <v>6</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="D7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="32" x14ac:dyDescent="0.2">
@@ -601,10 +601,10 @@
         <v>7</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>27</v>
+        <v>48</v>
       </c>
       <c r="D8" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="48" x14ac:dyDescent="0.2">
@@ -615,10 +615,10 @@
         <v>8</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D9" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="32" x14ac:dyDescent="0.2">
@@ -629,10 +629,10 @@
         <v>9</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D10" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="48" x14ac:dyDescent="0.2">
@@ -643,7 +643,7 @@
         <v>10</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="32" x14ac:dyDescent="0.2">
@@ -654,10 +654,10 @@
         <v>11</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="32" x14ac:dyDescent="0.2">
@@ -668,10 +668,10 @@
         <v>12</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D13" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="48" x14ac:dyDescent="0.2">
@@ -682,10 +682,10 @@
         <v>13</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D14" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -704,7 +704,7 @@
         <v>15</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="32" x14ac:dyDescent="0.2">
@@ -715,7 +715,7 @@
         <v>16</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="48" x14ac:dyDescent="0.2">
@@ -726,10 +726,10 @@
         <v>17</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D18" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="32" x14ac:dyDescent="0.2">
@@ -737,13 +737,13 @@
         <v>15</v>
       </c>
       <c r="B19" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D19" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>